<commit_message>
Add images to failed test cases and time to report
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/SauceDemoItems.xlsx
+++ b/src/test/resources/testdata/SauceDemoItems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cecilia\Computacion\Java\Wize-Demo\javaselenium_poc\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1932FA4-5C03-4C10-9BA1-A19B222C98A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568749CC-4FD2-49D2-9171-441402741CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4908" yWindow="1644" windowWidth="17280" windowHeight="8964" xr2:uid="{D7C30793-12F3-4155-A6AE-E0A54C01DF6E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>$29.99</t>
+  </si>
+  <si>
+    <t>Sauce Labs Bike Light</t>
+  </si>
+  <si>
+    <t>A red light isn't the desired state in testing but it sure helps when riding your bike at night. Water-resistant with 3 lighting modes, 1 AAA battery included.</t>
+  </si>
+  <si>
+    <t>$9.99</t>
   </si>
 </sst>
 </file>
@@ -97,9 +106,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -415,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03336F1A-9FFA-48AD-83E1-545B7E3A02B6}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,6 +459,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>